<commit_message>
CP02PMCO Cal and Ingest Sheet
Checked Cal and ingest sheets, had to correct ADCPT reference
designators for deployment 1 telemetered and recovered from RII01-01 to
RII01-02.  Created D3 csv
</commit_message>
<xml_diff>
--- a/CP02PMCO/Omaha_Cal_Info_CP02PMCO_00003.xlsx
+++ b/CP02PMCO/Omaha_Cal_Info_CP02PMCO_00003.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="10720" windowWidth="25980" windowHeight="11280" tabRatio="377"/>
+    <workbookView xWindow="11280" yWindow="10725" windowWidth="25980" windowHeight="11280" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -363,6 +363,7 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -395,12 +396,14 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -956,7 +959,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -967,18 +970,18 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="11" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30">
+    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1013,7 +1016,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="20" customFormat="1" ht="15">
+    <row r="2" spans="1:11" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>11</v>
       </c>
@@ -1062,21 +1065,21 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.5" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" customWidth="1"/>
     <col min="7" max="7" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30">
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1096,7 +1099,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>61</v>
       </c>
@@ -1120,7 +1123,7 @@
       </c>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>61</v>
       </c>
@@ -1142,7 +1145,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>61</v>
       </c>
@@ -1164,7 +1167,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1174,7 +1177,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>60</v>
       </c>
@@ -1194,10 +1197,10 @@
       </c>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D7" s="14"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
@@ -1221,7 +1224,7 @@
       </c>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
@@ -1243,7 +1246,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
@@ -1265,7 +1268,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
@@ -1289,7 +1292,7 @@
       </c>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>19</v>
       </c>
@@ -1313,7 +1316,7 @@
       </c>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
@@ -1337,7 +1340,7 @@
       </c>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
@@ -1361,7 +1364,7 @@
       </c>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>19</v>
       </c>
@@ -1385,7 +1388,7 @@
       </c>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -1395,7 +1398,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>32</v>
       </c>
@@ -1417,7 +1420,7 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>32</v>
       </c>
@@ -1439,7 +1442,7 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1449,7 +1452,7 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
         <v>68</v>
       </c>
@@ -1471,7 +1474,7 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
         <v>68</v>
       </c>
@@ -1493,7 +1496,7 @@
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1503,7 +1506,7 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>35</v>
       </c>
@@ -1527,7 +1530,7 @@
       </c>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>35</v>
       </c>
@@ -1551,7 +1554,7 @@
       </c>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>35</v>
       </c>
@@ -1575,7 +1578,7 @@
       </c>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>35</v>
       </c>
@@ -1599,7 +1602,7 @@
       </c>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>35</v>
       </c>
@@ -1623,7 +1626,7 @@
       </c>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>35</v>
       </c>
@@ -1647,7 +1650,7 @@
       </c>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>35</v>
       </c>
@@ -1671,7 +1674,7 @@
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>35</v>
       </c>
@@ -1695,7 +1698,7 @@
       </c>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>35</v>
       </c>
@@ -1719,7 +1722,7 @@
       </c>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>35</v>
       </c>
@@ -1743,7 +1746,7 @@
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1753,7 +1756,7 @@
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>52</v>
       </c>
@@ -1777,7 +1780,7 @@
       </c>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>52</v>
       </c>
@@ -1801,7 +1804,7 @@
       </c>
       <c r="H35" s="6"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1811,7 +1814,7 @@
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>59</v>
       </c>
@@ -1829,10 +1832,10 @@
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D38" s="24"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
Pioneer Profiler Mooring Cal and Ingest sheet
corrections to CP04OSPM, CP02PMUO, CP02PMUI, and CP02PMCO cal sheets,
made ingest CSV where needed.

Corrected LAT Lon format, reference designators, and file paths where
necessary
</commit_message>
<xml_diff>
--- a/CP02PMCO/Omaha_Cal_Info_CP02PMCO_00003.xlsx
+++ b/CP02PMCO/Omaha_Cal_Info_CP02PMCO_00003.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\Ingest sheets\ingestion-csvs\CP02PMCO\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="11280" yWindow="10725" windowWidth="25980" windowHeight="11280" tabRatio="377"/>
   </bookViews>
@@ -30,7 +35,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$78</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$401</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -254,9 +259,6 @@
     <t>CP02PMCO-00003</t>
   </si>
   <si>
-    <t>70° 52.764’ W</t>
-  </si>
-  <si>
     <t>AT-27</t>
   </si>
   <si>
@@ -275,10 +277,13 @@
     <t>43-2628</t>
   </si>
   <si>
-    <t>PMCO-00003-MOPAK</t>
-  </si>
-  <si>
-    <t>40° 5.801’ N</t>
+    <t>40°5.801'N</t>
+  </si>
+  <si>
+    <t>70°52.764'W</t>
+  </si>
+  <si>
+    <t>CP02PMCO-MOPAK</t>
   </si>
 </sst>
 </file>
@@ -288,7 +293,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -405,6 +410,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -514,7 +525,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -596,6 +607,9 @@
     </xf>
     <xf numFmtId="11" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="23">
@@ -959,7 +973,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -967,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,7 +995,7 @@
     <col min="4" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1016,7 +1030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>11</v>
       </c>
@@ -1036,18 +1050,26 @@
         <v>42291</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I2" s="15">
         <v>147</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K2" s="19"/>
+      <c r="L2" s="34">
+        <f>((LEFT(G2,(FIND("°",G2,1)-1)))+(MID(G2,(FIND("°",G2,1)+1),(FIND("'",G2,1))-(FIND("°",G2,1)+1))/60))*(IF(RIGHT(G2,1)="N",1,-1))</f>
+        <v>40.096683333333331</v>
+      </c>
+      <c r="M2" s="34">
+        <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="E",1,-1))</f>
+        <v>-70.879400000000004</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1065,7 +1087,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,7 +1141,7 @@
         <v>127000</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H2" s="6"/>
     </row>
@@ -1188,7 +1210,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
@@ -1211,7 +1233,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>20</v>
@@ -1235,7 +1257,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>17</v>
@@ -1257,7 +1279,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>18</v>
@@ -1279,7 +1301,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>22</v>
@@ -1303,7 +1325,7 @@
         <v>3</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>24</v>
@@ -1327,7 +1349,7 @@
         <v>3</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>26</v>
@@ -1351,7 +1373,7 @@
         <v>3</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>28</v>
@@ -1375,7 +1397,7 @@
         <v>3</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>30</v>
@@ -1454,7 +1476,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>62</v>
@@ -1476,7 +1498,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>62</v>
@@ -1825,7 +1847,7 @@
         <v>3</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="7"/>
@@ -1846,7 +1868,7 @@
         <v>3</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="7"/>

</xml_diff>